<commit_message>
Correct errors in insert_compound_names
</commit_message>
<xml_diff>
--- a/data_extraction/test/files/compounded_names.xlsx
+++ b/data_extraction/test/files/compounded_names.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Nombre</t>
   </si>
@@ -43,9 +43,6 @@
   </si>
   <si>
     <t>JAVIER</t>
-  </si>
-  <si>
-    <t>Calculation</t>
   </si>
 </sst>
 </file>
@@ -81,8 +78,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -414,86 +412,97 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="23.33203125" customWidth="1"/>
-    <col min="3" max="3" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="3" width="23.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2">
         <v>10</v>
       </c>
-      <c r="C2">
-        <f>B2/46464053</f>
-        <v>2.1522014018019479E-7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3">
         <v>10</v>
       </c>
-      <c r="C3">
-        <f>B3/46464053</f>
-        <v>2.1522014018019479E-7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
+    <row r="5" spans="1:4">
+      <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
-      <c r="A6" t="s">
+    <row r="6" spans="1:4">
+      <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
-      <c r="A7" t="s">
+    <row r="7" spans="1:4">
+      <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7">
         <v>10</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A7:C7"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>